<commit_message>
fixed error in external Dpitch calculation
</commit_message>
<xml_diff>
--- a/BSPthread/BSPthread.xlsx
+++ b/BSPthread/BSPthread.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Projects/Waterrockets/Bottle2GardenaAdapterWithFins/BSPthread/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99D6C33-DC23-2B41-98BE-3E4B45D3B41A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED2432B-87F7-2541-BB0C-32F1685F3B48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12360" yWindow="460" windowWidth="26040" windowHeight="21140" xr2:uid="{46C58C85-D7E3-B144-AD74-40B7546B4D31}"/>
+    <workbookView xWindow="14520" yWindow="460" windowWidth="23880" windowHeight="21140" xr2:uid="{46C58C85-D7E3-B144-AD74-40B7546B4D31}"/>
   </bookViews>
   <sheets>
     <sheet name="BSPP thread" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,13 @@
     <definedName name="cinternal">'BSPP thread'!$R$1</definedName>
     <definedName name="deg">meta!$B$2</definedName>
     <definedName name="phi">meta!$B$3</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'BSPP thread'!$R$1</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'BSPP thread'!$Y$1</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'BSPP thread'!$R$1</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'BSPP thread'!$R$1</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'BSPP thread'!$Y$1</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'BSPP thread'!$Y$1</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
@@ -36,7 +36,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'BSPP thread'!$P$27</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'BSPP thread'!$Y$27</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
@@ -215,7 +215,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -744,6 +744,16 @@
     <xf numFmtId="10" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -762,16 +772,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -957,7 +957,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Dminor for internal:</a:t>
+            <a:t>Dminor for external:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1283,11 +1283,11 @@
   <dimension ref="A1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O3" sqref="O3"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" bestFit="1" customWidth="1"/>
@@ -1312,52 +1312,52 @@
     <col min="22" max="22" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:25" ht="17" thickBot="1">
+      <c r="A1" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="57" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="58"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="58" t="s">
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="58"/>
-      <c r="J1" s="57" t="s">
+      <c r="I1" s="62"/>
+      <c r="J1" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="59"/>
+      <c r="K1" s="63"/>
       <c r="L1" s="17"/>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="63">
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="54">
         <v>0.27205047575333813</v>
       </c>
-      <c r="T1" s="54" t="s">
+      <c r="T1" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="63">
-        <v>0.24522234485775363</v>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="54">
+        <v>0.29097758142887981</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="110" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="110" thickBot="1">
       <c r="A2" s="25" t="s">
         <v>27</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25">
       <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>0.14099956301655503</v>
       </c>
       <c r="Q3" s="44">
-        <f>M3+C3*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" ref="Q3:Q26" si="1">M3+C3*5/12/TAN(phi/2)*1.05</f>
         <v>7.9577697202587458</v>
       </c>
       <c r="R3" s="33" t="b">
@@ -1490,31 +1490,31 @@
         <v>1</v>
       </c>
       <c r="T3" s="32">
-        <f t="shared" ref="T3:T26" si="1">$E3+0.5*$F3</f>
-        <v>7.1955</v>
+        <f>$E3+0.5*$G3</f>
+        <v>7.0885000000000007</v>
       </c>
       <c r="U3" s="49">
-        <f>MIN(T3-(E3+G3), E3-T3)/G3</f>
+        <f>-MIN(T3-(E3+G3), E3-T3)/G3</f>
         <v>0.49999999999999684</v>
       </c>
       <c r="V3" s="32">
-        <f>T3-C3*5/12/TAN(phi/2)*1.05</f>
-        <v>6.4332302797412542</v>
+        <f t="shared" ref="V3:V26" si="2">T3-C3*5/12/TAN(phi/2)*1.05</f>
+        <v>6.3262302797412548</v>
       </c>
       <c r="W3" s="38" t="b">
         <f>V3&lt;=H3</f>
         <v>1</v>
       </c>
       <c r="X3" s="44">
-        <f t="shared" ref="X3:X26" si="2">T3+C3*2*cexternal</f>
-        <v>7.6403333335719648</v>
+        <f t="shared" ref="X3:X26" si="3">T3+C3*2*cexternal</f>
+        <v>7.6163333327119886</v>
       </c>
       <c r="Y3" s="39">
         <f>MIN(X3-(J3+K3), J3-X3)</f>
-        <v>8.2666666428035107E-2</v>
+        <v>0.10666666728801122</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>0.107</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" ref="G4:G26" si="3">-F4</f>
+        <f t="shared" ref="G4:G26" si="4">-F4</f>
         <v>-0.107</v>
       </c>
       <c r="H4" s="15">
@@ -1551,11 +1551,11 @@
       </c>
       <c r="L4" s="9"/>
       <c r="M4" s="34">
-        <f t="shared" ref="M4:M26" si="4">$E4+0.5*$F4</f>
+        <f t="shared" ref="M4:M26" si="5">$E4+0.5*$F4</f>
         <v>9.2004999999999999</v>
       </c>
       <c r="N4" s="50">
-        <f t="shared" ref="N4:N26" si="5">MIN(M4-E4,E4+F4-M4)/F4</f>
+        <f t="shared" ref="N4:N26" si="6">MIN(M4-E4,E4+F4-M4)/F4</f>
         <v>0.49999999999999684</v>
       </c>
       <c r="O4" s="34">
@@ -1563,43 +1563,43 @@
         <v>8.7070004369834439</v>
       </c>
       <c r="P4" s="40">
-        <f t="shared" ref="P4:P26" si="6">MIN(O4-H4, H4+I4-O4)</f>
+        <f t="shared" ref="P4:P26" si="7">MIN(O4-H4, H4+I4-O4)</f>
         <v>0.14099956301655681</v>
       </c>
       <c r="Q4" s="45">
-        <f>M4+C4*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>9.9627697202587449</v>
       </c>
       <c r="R4" s="35" t="b">
-        <f t="shared" ref="R4:R26" si="7">Q4&gt;=J4</f>
+        <f t="shared" ref="R4:R26" si="8">Q4&gt;=J4</f>
         <v>1</v>
       </c>
       <c r="T4" s="34">
-        <f t="shared" si="1"/>
-        <v>9.2004999999999999</v>
+        <f t="shared" ref="T4:T26" si="9">$E4+0.5*$G4</f>
+        <v>9.0935000000000006</v>
       </c>
       <c r="U4" s="50">
-        <f t="shared" ref="U4:U26" si="8">MIN(T4-(E4+G4), E4-T4)/G4</f>
+        <f t="shared" ref="U4:U26" si="10">-MIN(T4-(E4+G4), E4-T4)/G4</f>
         <v>0.49999999999999684</v>
       </c>
       <c r="V4" s="34">
-        <f>T4-C4*5/12/TAN(phi/2)*1.05</f>
-        <v>8.4382302797412549</v>
+        <f t="shared" si="2"/>
+        <v>8.3312302797412556</v>
       </c>
       <c r="W4" s="52" t="b">
-        <f t="shared" ref="W4:W26" si="9">V4&lt;=H4</f>
+        <f t="shared" ref="W4:W26" si="11">V4&lt;=H4</f>
         <v>1</v>
       </c>
       <c r="X4" s="45">
-        <f t="shared" si="2"/>
-        <v>9.6453333335719655</v>
+        <f t="shared" si="3"/>
+        <v>9.6213333327119877</v>
       </c>
       <c r="Y4" s="40">
-        <f t="shared" ref="Y4:Y26" si="10">MIN(X4-(J4+K4), J4-X4)</f>
-        <v>8.2666666428034219E-2</v>
+        <f t="shared" ref="Y4:Y26" si="12">MIN(X4-(J4+K4), J4-X4)</f>
+        <v>0.10666666728801211</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>0.125</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.125</v>
       </c>
       <c r="H5" s="15">
@@ -1636,11 +1636,11 @@
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12.3635</v>
       </c>
       <c r="N5" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="O5" s="34">
@@ -1648,43 +1648,43 @@
         <v>11.636037027835574</v>
       </c>
       <c r="P5" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.19103702783557353</v>
       </c>
       <c r="Q5" s="45">
-        <f>M5+C5*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>13.487154482895196</v>
       </c>
       <c r="R5" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T5" s="34">
-        <f t="shared" si="1"/>
-        <v>12.3635</v>
+        <f t="shared" si="9"/>
+        <v>12.2385</v>
       </c>
       <c r="U5" s="50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="V5" s="34">
-        <f>T5-C5*5/12/TAN(phi/2)*1.05</f>
-        <v>11.239845517104804</v>
+        <f t="shared" si="2"/>
+        <v>11.114845517104804</v>
       </c>
       <c r="W5" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X5" s="45">
-        <f t="shared" si="2"/>
-        <v>13.019224550149634</v>
+        <f t="shared" si="3"/>
+        <v>13.016574052740825</v>
       </c>
       <c r="Y5" s="40">
-        <f t="shared" si="10"/>
-        <v>0.11222455014963373</v>
+        <f t="shared" si="12"/>
+        <v>0.10957405274082532</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>0.125</v>
       </c>
       <c r="G6" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.125</v>
       </c>
       <c r="H6" s="15">
@@ -1721,11 +1721,11 @@
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>15.868499999999999</v>
       </c>
       <c r="N6" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="O6" s="34">
@@ -1733,43 +1733,43 @@
         <v>15.141037027835573</v>
       </c>
       <c r="P6" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.19103702783557353</v>
       </c>
       <c r="Q6" s="45">
-        <f>M6+C6*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>16.992154482895195</v>
       </c>
       <c r="R6" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T6" s="34">
-        <f t="shared" si="1"/>
-        <v>15.868499999999999</v>
+        <f t="shared" si="9"/>
+        <v>15.743499999999999</v>
       </c>
       <c r="U6" s="50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="V6" s="34">
-        <f>T6-C6*5/12/TAN(phi/2)*1.05</f>
-        <v>14.744845517104803</v>
+        <f t="shared" si="2"/>
+        <v>14.619845517104803</v>
       </c>
       <c r="W6" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X6" s="45">
-        <f t="shared" si="2"/>
-        <v>16.524224550149633</v>
+        <f t="shared" si="3"/>
+        <v>16.521574052740824</v>
       </c>
       <c r="Y6" s="40">
-        <f t="shared" si="10"/>
-        <v>0.11222455014963373</v>
+        <f t="shared" si="12"/>
+        <v>0.10957405274082532</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="G7" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.14199999999999999</v>
       </c>
       <c r="H7" s="15">
@@ -1806,11 +1806,11 @@
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>19.864000000000001</v>
       </c>
       <c r="N7" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999998562</v>
       </c>
       <c r="O7" s="34">
@@ -1818,43 +1818,43 @@
         <v>18.877000873966889</v>
       </c>
       <c r="P7" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.24600087396688863</v>
       </c>
       <c r="Q7" s="45">
-        <f>M7+C7*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>21.388539440517491</v>
       </c>
       <c r="R7" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T7" s="34">
-        <f t="shared" si="1"/>
-        <v>19.864000000000001</v>
+        <f t="shared" si="9"/>
+        <v>19.721999999999998</v>
       </c>
       <c r="U7" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000001066</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999998562</v>
       </c>
       <c r="V7" s="34">
-        <f>T7-C7*5/12/TAN(phi/2)*1.05</f>
-        <v>18.339460559482511</v>
+        <f t="shared" si="2"/>
+        <v>18.197460559482508</v>
       </c>
       <c r="W7" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X7" s="45">
-        <f t="shared" si="2"/>
-        <v>20.753666667143932</v>
+        <f t="shared" si="3"/>
+        <v>20.777666665423972</v>
       </c>
       <c r="Y7" s="40">
-        <f t="shared" si="10"/>
-        <v>8.2666667143932671E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.10666666542397252</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.14199999999999999</v>
       </c>
       <c r="H8" s="15">
@@ -1891,11 +1891,11 @@
       </c>
       <c r="L8" s="9"/>
       <c r="M8" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>21.82</v>
       </c>
       <c r="N8" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999998562</v>
       </c>
       <c r="O8" s="34">
@@ -1903,43 +1903,43 @@
         <v>20.833000873966888</v>
       </c>
       <c r="P8" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.24600087396688863</v>
       </c>
       <c r="Q8" s="45">
-        <f>M8+C8*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>23.344539440517494</v>
       </c>
       <c r="R8" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T8" s="34">
-        <f t="shared" si="1"/>
-        <v>21.82</v>
+        <f t="shared" si="9"/>
+        <v>21.677999999999997</v>
       </c>
       <c r="U8" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000001066</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999998562</v>
       </c>
       <c r="V8" s="34">
-        <f>T8-C8*5/12/TAN(phi/2)*1.05</f>
-        <v>20.295460559482507</v>
+        <f t="shared" si="2"/>
+        <v>20.153460559482504</v>
       </c>
       <c r="W8" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X8" s="45">
-        <f t="shared" si="2"/>
-        <v>22.709666667143932</v>
+        <f t="shared" si="3"/>
+        <v>22.733666665423975</v>
       </c>
       <c r="Y8" s="40">
-        <f t="shared" si="10"/>
-        <v>8.2666667143929118E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.10666666542397252</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.14199999999999999</v>
       </c>
       <c r="H9" s="15">
@@ -1976,11 +1976,11 @@
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>25.35</v>
       </c>
       <c r="N9" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999998562</v>
       </c>
       <c r="O9" s="34">
@@ -1988,43 +1988,43 @@
         <v>24.36300087396689</v>
       </c>
       <c r="P9" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.24600087396688863</v>
       </c>
       <c r="Q9" s="45">
-        <f>M9+C9*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>26.874539440517495</v>
       </c>
       <c r="R9" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T9" s="34">
-        <f t="shared" si="1"/>
-        <v>25.35</v>
+        <f t="shared" si="9"/>
+        <v>25.207999999999998</v>
       </c>
       <c r="U9" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000001066</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999998562</v>
       </c>
       <c r="V9" s="34">
-        <f>T9-C9*5/12/TAN(phi/2)*1.05</f>
-        <v>23.825460559482508</v>
+        <f t="shared" si="2"/>
+        <v>23.683460559482505</v>
       </c>
       <c r="W9" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X9" s="45">
-        <f t="shared" si="2"/>
-        <v>26.239666667143933</v>
+        <f t="shared" si="3"/>
+        <v>26.263666665423976</v>
       </c>
       <c r="Y9" s="40">
-        <f t="shared" si="10"/>
-        <v>8.2666667143932671E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.10666666542397607</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.14199999999999999</v>
       </c>
       <c r="H10" s="15">
@@ -2061,11 +2061,11 @@
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.110000000000003</v>
       </c>
       <c r="N10" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999998562</v>
       </c>
       <c r="O10" s="34">
@@ -2073,43 +2073,43 @@
         <v>28.123000873966891</v>
       </c>
       <c r="P10" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.24600087396689219</v>
       </c>
       <c r="Q10" s="45">
-        <f>M10+C10*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>30.634539440517493</v>
       </c>
       <c r="R10" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T10" s="34">
-        <f t="shared" si="1"/>
-        <v>29.110000000000003</v>
+        <f t="shared" si="9"/>
+        <v>28.968</v>
       </c>
       <c r="U10" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000001066</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999998562</v>
       </c>
       <c r="V10" s="34">
-        <f>T10-C10*5/12/TAN(phi/2)*1.05</f>
-        <v>27.585460559482513</v>
+        <f t="shared" si="2"/>
+        <v>27.44346055948251</v>
       </c>
       <c r="W10" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X10" s="45">
-        <f t="shared" si="2"/>
-        <v>29.999666667143934</v>
+        <f t="shared" si="3"/>
+        <v>30.023666665423974</v>
       </c>
       <c r="Y10" s="40">
-        <f t="shared" si="10"/>
-        <v>8.2666667143932671E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.10666666542397252</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>0.18</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.18</v>
       </c>
       <c r="H11" s="15">
@@ -2146,11 +2146,11 @@
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>31.86</v>
       </c>
       <c r="N11" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999999922</v>
       </c>
       <c r="O11" s="34">
@@ -2158,43 +2158,43 @@
         <v>30.603670902971082</v>
       </c>
       <c r="P11" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.31267090297108169</v>
       </c>
       <c r="Q11" s="45">
-        <f>M11+C11*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>33.800552132389683</v>
       </c>
       <c r="R11" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T11" s="34">
-        <f t="shared" si="1"/>
-        <v>31.86</v>
+        <f t="shared" si="9"/>
+        <v>31.68</v>
       </c>
       <c r="U11" s="50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.49999999999999922</v>
       </c>
       <c r="V11" s="34">
-        <f>T11-C11*5/12/TAN(phi/2)*1.05</f>
-        <v>29.919447867610316</v>
+        <f t="shared" si="2"/>
+        <v>29.739447867610316</v>
       </c>
       <c r="W11" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X11" s="45">
-        <f t="shared" si="2"/>
-        <v>32.992436788553107</v>
+        <f t="shared" si="3"/>
+        <v>33.023734471038566</v>
       </c>
       <c r="Y11" s="40">
-        <f t="shared" si="10"/>
-        <v>0.10343678855310401</v>
+        <f t="shared" si="12"/>
+        <v>0.13473447103856273</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>0.18</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.18</v>
       </c>
       <c r="H12" s="15">
@@ -2231,11 +2231,11 @@
       </c>
       <c r="L12" s="9"/>
       <c r="M12" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>36.508000000000003</v>
       </c>
       <c r="N12" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999997952</v>
       </c>
       <c r="O12" s="34">
@@ -2243,43 +2243,43 @@
         <v>35.251670902971085</v>
       </c>
       <c r="P12" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.31267090297108524</v>
       </c>
       <c r="Q12" s="45">
-        <f>M12+C12*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>38.448552132389686</v>
       </c>
       <c r="R12" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T12" s="34">
-        <f t="shared" si="1"/>
-        <v>36.508000000000003</v>
+        <f t="shared" si="9"/>
+        <v>36.327999999999996</v>
       </c>
       <c r="U12" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000001898</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999997952</v>
       </c>
       <c r="V12" s="34">
-        <f>T12-C12*5/12/TAN(phi/2)*1.05</f>
-        <v>34.567447867610319</v>
+        <f t="shared" si="2"/>
+        <v>34.387447867610312</v>
       </c>
       <c r="W12" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X12" s="45">
-        <f t="shared" si="2"/>
-        <v>37.64043678855311</v>
+        <f t="shared" si="3"/>
+        <v>37.671734471038562</v>
       </c>
       <c r="Y12" s="40">
-        <f t="shared" si="10"/>
-        <v>0.10343678855311111</v>
+        <f t="shared" si="12"/>
+        <v>0.13473447103856273</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>0.18</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.18</v>
       </c>
       <c r="H13" s="15">
@@ -2316,11 +2316,11 @@
       </c>
       <c r="L13" s="9"/>
       <c r="M13" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>40.521000000000001</v>
       </c>
       <c r="N13" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999997952</v>
       </c>
       <c r="O13" s="34">
@@ -2328,43 +2328,43 @@
         <v>39.264670902971083</v>
       </c>
       <c r="P13" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.31267090297108524</v>
       </c>
       <c r="Q13" s="45">
-        <f>M13+C13*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>42.461552132389684</v>
       </c>
       <c r="R13" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T13" s="34">
-        <f t="shared" si="1"/>
-        <v>40.521000000000001</v>
+        <f t="shared" si="9"/>
+        <v>40.340999999999994</v>
       </c>
       <c r="U13" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000001898</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999997952</v>
       </c>
       <c r="V13" s="34">
-        <f>T13-C13*5/12/TAN(phi/2)*1.05</f>
-        <v>38.580447867610317</v>
+        <f t="shared" si="2"/>
+        <v>38.40044786761031</v>
       </c>
       <c r="W13" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X13" s="45">
-        <f t="shared" si="2"/>
-        <v>41.653436788553108</v>
+        <f t="shared" si="3"/>
+        <v>41.68473447103856</v>
       </c>
       <c r="Y13" s="40">
-        <f t="shared" si="10"/>
-        <v>0.10343678855311111</v>
+        <f t="shared" si="12"/>
+        <v>0.13473447103856273</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>0.18</v>
       </c>
       <c r="G14" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.18</v>
       </c>
       <c r="H14" s="15">
@@ -2401,11 +2401,11 @@
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>46.414000000000001</v>
       </c>
       <c r="N14" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999997952</v>
       </c>
       <c r="O14" s="34">
@@ -2413,43 +2413,43 @@
         <v>45.157670902971084</v>
       </c>
       <c r="P14" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.31267090297108524</v>
       </c>
       <c r="Q14" s="45">
-        <f>M14+C14*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>48.354552132389685</v>
       </c>
       <c r="R14" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T14" s="34">
-        <f t="shared" si="1"/>
-        <v>46.414000000000001</v>
+        <f t="shared" si="9"/>
+        <v>46.233999999999995</v>
       </c>
       <c r="U14" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000001898</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999997952</v>
       </c>
       <c r="V14" s="34">
-        <f>T14-C14*5/12/TAN(phi/2)*1.05</f>
-        <v>44.473447867610318</v>
+        <f t="shared" si="2"/>
+        <v>44.293447867610311</v>
       </c>
       <c r="W14" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X14" s="45">
-        <f t="shared" si="2"/>
-        <v>47.546436788553109</v>
+        <f t="shared" si="3"/>
+        <v>47.577734471038561</v>
       </c>
       <c r="Y14" s="40">
-        <f t="shared" si="10"/>
-        <v>0.10343678855311111</v>
+        <f t="shared" si="12"/>
+        <v>0.13473447103856273</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>0.18</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.18</v>
       </c>
       <c r="H15" s="15">
@@ -2486,11 +2486,11 @@
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>52.357000000000006</v>
       </c>
       <c r="N15" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999997952</v>
       </c>
       <c r="O15" s="34">
@@ -2498,43 +2498,43 @@
         <v>51.100670902971089</v>
       </c>
       <c r="P15" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.31267090297109235</v>
       </c>
       <c r="Q15" s="45">
-        <f>M15+C15*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>54.29755213238969</v>
       </c>
       <c r="R15" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T15" s="34">
-        <f t="shared" si="1"/>
-        <v>52.357000000000006</v>
+        <f t="shared" si="9"/>
+        <v>52.177</v>
       </c>
       <c r="U15" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000001898</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999997952</v>
       </c>
       <c r="V15" s="34">
-        <f>T15-C15*5/12/TAN(phi/2)*1.05</f>
-        <v>50.416447867610323</v>
+        <f t="shared" si="2"/>
+        <v>50.236447867610316</v>
       </c>
       <c r="W15" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X15" s="45">
-        <f t="shared" si="2"/>
-        <v>53.489436788553114</v>
+        <f t="shared" si="3"/>
+        <v>53.520734471038566</v>
       </c>
       <c r="Y15" s="40">
-        <f t="shared" si="10"/>
-        <v>0.10343678855311111</v>
+        <f t="shared" si="12"/>
+        <v>0.13473447103856273</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>0.18</v>
       </c>
       <c r="G16" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.18</v>
       </c>
       <c r="H16" s="15">
@@ -2571,11 +2571,11 @@
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>58.225000000000001</v>
       </c>
       <c r="N16" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999997952</v>
       </c>
       <c r="O16" s="34">
@@ -2583,43 +2583,43 @@
         <v>56.968670902971084</v>
       </c>
       <c r="P16" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.31267090297108524</v>
       </c>
       <c r="Q16" s="45">
-        <f>M16+C16*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>60.165552132389685</v>
       </c>
       <c r="R16" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T16" s="34">
-        <f t="shared" si="1"/>
-        <v>58.225000000000001</v>
+        <f t="shared" si="9"/>
+        <v>58.044999999999995</v>
       </c>
       <c r="U16" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000001898</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999997952</v>
       </c>
       <c r="V16" s="34">
-        <f>T16-C16*5/12/TAN(phi/2)*1.05</f>
-        <v>56.284447867610318</v>
+        <f t="shared" si="2"/>
+        <v>56.104447867610311</v>
       </c>
       <c r="W16" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X16" s="45">
-        <f t="shared" si="2"/>
-        <v>59.357436788553109</v>
+        <f t="shared" si="3"/>
+        <v>59.388734471038561</v>
       </c>
       <c r="Y16" s="40">
-        <f t="shared" si="10"/>
-        <v>0.10343678855311111</v>
+        <f t="shared" si="12"/>
+        <v>0.13473447103856273</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>0.217</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.217</v>
       </c>
       <c r="H17" s="15">
@@ -2656,11 +2656,11 @@
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>64.339500000000001</v>
       </c>
       <c r="N17" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="O17" s="34">
@@ -2668,43 +2668,43 @@
         <v>63.083170902971084</v>
       </c>
       <c r="P17" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30882909702891936</v>
       </c>
       <c r="Q17" s="45">
-        <f>M17+C17*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>66.280052132389685</v>
       </c>
       <c r="R17" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T17" s="34">
-        <f t="shared" si="1"/>
-        <v>64.339500000000001</v>
+        <f t="shared" si="9"/>
+        <v>64.122499999999988</v>
       </c>
       <c r="U17" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000002986</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999996436</v>
       </c>
       <c r="V17" s="34">
-        <f>T17-C17*5/12/TAN(phi/2)*1.05</f>
-        <v>62.398947867610318</v>
+        <f t="shared" si="2"/>
+        <v>62.181947867610305</v>
       </c>
       <c r="W17" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X17" s="45">
-        <f t="shared" si="2"/>
-        <v>65.471936788553108</v>
+        <f t="shared" si="3"/>
+        <v>65.466234471038561</v>
       </c>
       <c r="Y17" s="40">
-        <f t="shared" si="10"/>
-        <v>0.19593678855311225</v>
+        <f t="shared" si="12"/>
+        <v>0.19023447103856483</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>0.217</v>
       </c>
       <c r="G18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.217</v>
       </c>
       <c r="H18" s="15">
@@ -2741,11 +2741,11 @@
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.813500000000005</v>
       </c>
       <c r="N18" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="O18" s="34">
@@ -2753,43 +2753,43 @@
         <v>72.557170902971095</v>
       </c>
       <c r="P18" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30882909702890515</v>
       </c>
       <c r="Q18" s="45">
-        <f>M18+C18*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>75.754052132389688</v>
       </c>
       <c r="R18" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T18" s="34">
-        <f t="shared" si="1"/>
-        <v>73.813500000000005</v>
+        <f t="shared" si="9"/>
+        <v>73.596499999999992</v>
       </c>
       <c r="U18" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000002986</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999996436</v>
       </c>
       <c r="V18" s="34">
-        <f>T18-C18*5/12/TAN(phi/2)*1.05</f>
-        <v>71.872947867610321</v>
+        <f t="shared" si="2"/>
+        <v>71.655947867610308</v>
       </c>
       <c r="W18" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X18" s="45">
-        <f t="shared" si="2"/>
-        <v>74.945936788553112</v>
+        <f t="shared" si="3"/>
+        <v>74.940234471038565</v>
       </c>
       <c r="Y18" s="40">
-        <f t="shared" si="10"/>
-        <v>0.19593678855311225</v>
+        <f t="shared" si="12"/>
+        <v>0.19023447103856483</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>0.217</v>
       </c>
       <c r="G19" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.217</v>
       </c>
       <c r="H19" s="15">
@@ -2826,11 +2826,11 @@
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>80.163500000000013</v>
       </c>
       <c r="N19" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="O19" s="34">
@@ -2838,43 +2838,43 @@
         <v>78.907170902971103</v>
       </c>
       <c r="P19" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30882909702889094</v>
       </c>
       <c r="Q19" s="45">
-        <f>M19+C19*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>82.104052132389697</v>
       </c>
       <c r="R19" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T19" s="34">
-        <f t="shared" si="1"/>
-        <v>80.163500000000013</v>
+        <f t="shared" si="9"/>
+        <v>79.9465</v>
       </c>
       <c r="U19" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000002986</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999996436</v>
       </c>
       <c r="V19" s="34">
-        <f>T19-C19*5/12/TAN(phi/2)*1.05</f>
-        <v>78.22294786761033</v>
+        <f t="shared" si="2"/>
+        <v>78.005947867610317</v>
       </c>
       <c r="W19" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X19" s="45">
-        <f t="shared" si="2"/>
-        <v>81.295936788553121</v>
+        <f t="shared" si="3"/>
+        <v>81.290234471038573</v>
       </c>
       <c r="Y19" s="40">
-        <f t="shared" si="10"/>
-        <v>0.19593678855311225</v>
+        <f t="shared" si="12"/>
+        <v>0.19023447103856483</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>0.217</v>
       </c>
       <c r="G20" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.217</v>
       </c>
       <c r="H20" s="15">
@@ -2911,11 +2911,11 @@
       </c>
       <c r="L20" s="9"/>
       <c r="M20" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>86.513500000000008</v>
       </c>
       <c r="N20" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="O20" s="34">
@@ -2923,43 +2923,43 @@
         <v>85.257170902971097</v>
       </c>
       <c r="P20" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30882909702890515</v>
       </c>
       <c r="Q20" s="45">
-        <f>M20+C20*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>88.454052132389691</v>
       </c>
       <c r="R20" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T20" s="34">
-        <f t="shared" si="1"/>
-        <v>86.513500000000008</v>
+        <f t="shared" si="9"/>
+        <v>86.296499999999995</v>
       </c>
       <c r="U20" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000002986</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999996436</v>
       </c>
       <c r="V20" s="34">
-        <f>T20-C20*5/12/TAN(phi/2)*1.05</f>
-        <v>84.572947867610324</v>
+        <f t="shared" si="2"/>
+        <v>84.355947867610311</v>
       </c>
       <c r="W20" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X20" s="45">
-        <f t="shared" si="2"/>
-        <v>87.645936788553115</v>
+        <f t="shared" si="3"/>
+        <v>87.640234471038568</v>
       </c>
       <c r="Y20" s="40">
-        <f t="shared" si="10"/>
-        <v>0.19593678855311225</v>
+        <f t="shared" si="12"/>
+        <v>0.19023447103856483</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>0.217</v>
       </c>
       <c r="G21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.217</v>
       </c>
       <c r="H21" s="15">
@@ -2996,11 +2996,11 @@
       </c>
       <c r="L21" s="9"/>
       <c r="M21" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>98.959500000000006</v>
       </c>
       <c r="N21" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="O21" s="34">
@@ -3008,43 +3008,43 @@
         <v>97.703170902971095</v>
       </c>
       <c r="P21" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30882909702890515</v>
       </c>
       <c r="Q21" s="45">
-        <f>M21+C21*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>100.90005213238969</v>
       </c>
       <c r="R21" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T21" s="34">
-        <f t="shared" si="1"/>
-        <v>98.959500000000006</v>
+        <f t="shared" si="9"/>
+        <v>98.742499999999993</v>
       </c>
       <c r="U21" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000002986</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999996436</v>
       </c>
       <c r="V21" s="34">
-        <f>T21-C21*5/12/TAN(phi/2)*1.05</f>
-        <v>97.018947867610322</v>
+        <f t="shared" si="2"/>
+        <v>96.801947867610309</v>
       </c>
       <c r="W21" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X21" s="45">
-        <f t="shared" si="2"/>
-        <v>100.09193678855311</v>
+        <f t="shared" si="3"/>
+        <v>100.08623447103857</v>
       </c>
       <c r="Y21" s="40">
-        <f t="shared" si="10"/>
-        <v>0.19593678855311225</v>
+        <f t="shared" si="12"/>
+        <v>0.19023447103856483</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>0.217</v>
       </c>
       <c r="G22" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.217</v>
       </c>
       <c r="H22" s="15">
@@ -3081,11 +3081,11 @@
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>111.65950000000001</v>
       </c>
       <c r="N22" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="O22" s="34">
@@ -3093,43 +3093,43 @@
         <v>110.4031709029711</v>
       </c>
       <c r="P22" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30882909702890515</v>
       </c>
       <c r="Q22" s="45">
-        <f>M22+C22*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>113.60005213238969</v>
       </c>
       <c r="R22" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T22" s="34">
-        <f t="shared" si="1"/>
-        <v>111.65950000000001</v>
+        <f t="shared" si="9"/>
+        <v>111.4425</v>
       </c>
       <c r="U22" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000002986</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999996436</v>
       </c>
       <c r="V22" s="34">
-        <f>T22-C22*5/12/TAN(phi/2)*1.05</f>
-        <v>109.71894786761032</v>
+        <f t="shared" si="2"/>
+        <v>109.50194786761031</v>
       </c>
       <c r="W22" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X22" s="45">
-        <f t="shared" si="2"/>
-        <v>112.79193678855312</v>
+        <f t="shared" si="3"/>
+        <v>112.78623447103857</v>
       </c>
       <c r="Y22" s="40">
-        <f t="shared" si="10"/>
-        <v>0.19593678855311225</v>
+        <f t="shared" si="12"/>
+        <v>0.19023447103856483</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>0.217</v>
       </c>
       <c r="G23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.217</v>
       </c>
       <c r="H23" s="15">
@@ -3166,11 +3166,11 @@
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>124.35950000000001</v>
       </c>
       <c r="N23" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="O23" s="34">
@@ -3178,43 +3178,43 @@
         <v>123.1031709029711</v>
       </c>
       <c r="P23" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30882909702890515</v>
       </c>
       <c r="Q23" s="45">
-        <f>M23+C23*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>126.30005213238969</v>
       </c>
       <c r="R23" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T23" s="34">
-        <f t="shared" si="1"/>
-        <v>124.35950000000001</v>
+        <f t="shared" si="9"/>
+        <v>124.1425</v>
       </c>
       <c r="U23" s="50">
-        <f t="shared" si="8"/>
-        <v>0.50000000000002986</v>
+        <f t="shared" si="10"/>
+        <v>0.49999999999996436</v>
       </c>
       <c r="V23" s="34">
-        <f>T23-C23*5/12/TAN(phi/2)*1.05</f>
-        <v>122.41894786761033</v>
+        <f t="shared" si="2"/>
+        <v>122.20194786761031</v>
       </c>
       <c r="W23" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X23" s="45">
-        <f t="shared" si="2"/>
-        <v>125.49193678855312</v>
+        <f t="shared" si="3"/>
+        <v>125.48623447103857</v>
       </c>
       <c r="Y23" s="40">
-        <f t="shared" si="10"/>
-        <v>0.19593678855311225</v>
+        <f t="shared" si="12"/>
+        <v>0.19023447103856483</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>0.217</v>
       </c>
       <c r="G24" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.217</v>
       </c>
       <c r="H24" s="15">
@@ -3251,11 +3251,11 @@
       </c>
       <c r="L24" s="9"/>
       <c r="M24" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>137.05949999999999</v>
       </c>
       <c r="N24" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="O24" s="34">
@@ -3263,43 +3263,43 @@
         <v>135.80317090297106</v>
       </c>
       <c r="P24" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30882909702893357</v>
       </c>
       <c r="Q24" s="45">
-        <f>M24+C24*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>139.00005213238967</v>
       </c>
       <c r="R24" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T24" s="34">
-        <f t="shared" si="1"/>
-        <v>137.05949999999999</v>
+        <f t="shared" si="9"/>
+        <v>136.8425</v>
       </c>
       <c r="U24" s="50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="V24" s="34">
-        <f>T24-C24*5/12/TAN(phi/2)*1.05</f>
-        <v>135.1189478676103</v>
+        <f t="shared" si="2"/>
+        <v>134.90194786761032</v>
       </c>
       <c r="W24" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X24" s="45">
-        <f t="shared" si="2"/>
-        <v>138.19193678855308</v>
+        <f t="shared" si="3"/>
+        <v>138.18623447103857</v>
       </c>
       <c r="Y24" s="40">
-        <f t="shared" si="10"/>
-        <v>0.19593678855306962</v>
+        <f t="shared" si="12"/>
+        <v>0.19023447103856483</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>0.217</v>
       </c>
       <c r="G25" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.217</v>
       </c>
       <c r="H25" s="15">
@@ -3336,11 +3336,11 @@
       </c>
       <c r="L25" s="9"/>
       <c r="M25" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>149.7595</v>
       </c>
       <c r="N25" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="O25" s="34">
@@ -3348,43 +3348,43 @@
         <v>148.50317090297108</v>
       </c>
       <c r="P25" s="40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30882909702890515</v>
       </c>
       <c r="Q25" s="45">
-        <f>M25+C25*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>151.70005213238969</v>
       </c>
       <c r="R25" s="35" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T25" s="34">
-        <f t="shared" si="1"/>
-        <v>149.7595</v>
+        <f t="shared" si="9"/>
+        <v>149.54250000000002</v>
       </c>
       <c r="U25" s="50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="V25" s="34">
-        <f>T25-C25*5/12/TAN(phi/2)*1.05</f>
-        <v>147.81894786761032</v>
+        <f t="shared" si="2"/>
+        <v>147.60194786761033</v>
       </c>
       <c r="W25" s="52" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X25" s="45">
-        <f t="shared" si="2"/>
-        <v>150.8919367885531</v>
+        <f t="shared" si="3"/>
+        <v>150.88623447103859</v>
       </c>
       <c r="Y25" s="40">
-        <f t="shared" si="10"/>
-        <v>0.19593678855309804</v>
+        <f t="shared" si="12"/>
+        <v>0.19023447103859326</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="17" thickBot="1">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>0.217</v>
       </c>
       <c r="G26" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.217</v>
       </c>
       <c r="H26" s="16">
@@ -3421,11 +3421,11 @@
       </c>
       <c r="L26" s="9"/>
       <c r="M26" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>162.45949999999999</v>
       </c>
       <c r="N26" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="O26" s="36">
@@ -3433,43 +3433,43 @@
         <v>161.20317090297107</v>
       </c>
       <c r="P26" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30882909702893357</v>
       </c>
       <c r="Q26" s="46">
-        <f>M26+C26*5/12/TAN(phi/2)*1.05</f>
+        <f t="shared" si="1"/>
         <v>164.40005213238967</v>
       </c>
       <c r="R26" s="37" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T26" s="36">
-        <f t="shared" si="1"/>
-        <v>162.45949999999999</v>
+        <f t="shared" si="9"/>
+        <v>162.24250000000001</v>
       </c>
       <c r="U26" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.49999999999996436</v>
       </c>
       <c r="V26" s="36">
-        <f>T26-C26*5/12/TAN(phi/2)*1.05</f>
-        <v>160.51894786761031</v>
+        <f t="shared" si="2"/>
+        <v>160.30194786761032</v>
       </c>
       <c r="W26" s="53" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="X26" s="46">
-        <f t="shared" si="2"/>
-        <v>163.59193678855308</v>
+        <f t="shared" si="3"/>
+        <v>163.58623447103858</v>
       </c>
       <c r="Y26" s="41">
-        <f t="shared" si="10"/>
-        <v>0.19593678855306962</v>
+        <f t="shared" si="12"/>
+        <v>0.19023447103856483</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25">
       <c r="M27" t="s">
         <v>45</v>
       </c>
@@ -3498,10 +3498,10 @@
       </c>
       <c r="Y27" s="42">
         <f>MIN(Y3:Y26)</f>
-        <v>8.2666666428034219E-2</v>
+        <v>0.10666666542397252</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25">
       <c r="N28" s="30"/>
       <c r="R28" s="31"/>
     </row>
@@ -3531,9 +3531,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="10" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>31</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="29" customFormat="1">
       <c r="A2" s="29" t="s">
         <v>35</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>34</v>
       </c>

</xml_diff>